<commit_message>
Port skip and take to GetFlights
</commit_message>
<xml_diff>
--- a/Test/Test.VirtualRadar.Database.SQLite/EmbeddedTestData/BaseStationDatabaseTests.xlsx
+++ b/Test/Test.VirtualRadar.Database.SQLite/EmbeddedTestData/BaseStationDatabaseTests.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Callsigns" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="GetAircraftBy" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="GetFlights" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="GetFlightsRows" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="255">
   <si>
     <t xml:space="preserve">Callsign1</t>
   </si>
@@ -760,6 +761,33 @@
   </si>
   <si>
     <t xml:space="preserve">Jj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StartRow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EndRow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExpectedCount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExpectedRows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,2,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">999</t>
   </si>
 </sst>
 </file>
@@ -848,12 +876,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -870,6 +898,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -952,23 +984,23 @@
   </sheetPr>
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="2.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="2.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="2.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="2.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="2.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="2.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="5.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="2.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="2.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="257" min="19" style="1" width="9.14"/>
   </cols>
   <sheetData>
@@ -1307,7 +1339,7 @@
   <dimension ref="A1:AW5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2109,7 +2141,7 @@
   <dimension ref="A1:AI9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2132,7 +2164,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="13.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="12.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="7.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="7.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="8.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="2" width="12.85"/>
@@ -3116,4 +3148,218 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>